<commit_message>
add new recoded genome for more stringent / generalized testing; fix in pipeline for mispriming area mapping for reference genome
</commit_message>
<xml_diff>
--- a/tests/test_output/seg23_masc_order.xlsx
+++ b/tests/test_output/seg23_masc_order.xlsx
@@ -32,217 +32,217 @@
     <t>A01</t>
   </si>
   <si>
-    <t>seg23.1.d</t>
-  </si>
-  <si>
-    <t>TTTTTGTTGTTTTTACAGATTTCCCATACG</t>
+    <t>seg23.1.j.d</t>
+  </si>
+  <si>
+    <t>GACTTTTTACGAGGCAGATAAAATTTCTC</t>
   </si>
   <si>
     <t>A02</t>
   </si>
   <si>
-    <t>seg23.1.wt</t>
-  </si>
-  <si>
-    <t>TTTTTGTTGTTTTTACAGATTTCCCATTCT</t>
+    <t>seg23.2.j.d</t>
+  </si>
+  <si>
+    <t>AGGAGTAAATAAAAAACAAAGAGACACAACT</t>
   </si>
   <si>
     <t>A03</t>
   </si>
   <si>
-    <t>seg23.1.c</t>
-  </si>
-  <si>
-    <t>CCGCAAAAACAGACTCAGGTG</t>
+    <t>seg23.3.j.d</t>
+  </si>
+  <si>
+    <t>CGCTGGATTTTCGACTAAAGTTCTG</t>
   </si>
   <si>
     <t>A04</t>
   </si>
   <si>
-    <t>seg23.2.d</t>
-  </si>
-  <si>
-    <t>TATGGATATGCTAGCGGTCGATCTT</t>
+    <t>seg23.4.j.d</t>
+  </si>
+  <si>
+    <t>TCATCATTCTCAATCAGACAACTCGA</t>
   </si>
   <si>
     <t>A05</t>
   </si>
   <si>
-    <t>seg23.2.wt</t>
-  </si>
-  <si>
-    <t>GATGGATATGCTAGCGGTCGATTTA</t>
+    <t>seg23.5.j.d</t>
+  </si>
+  <si>
+    <t>GATGACTTACAAATGCTTAGCCAATGA</t>
   </si>
   <si>
     <t>A06</t>
   </si>
   <si>
-    <t>seg23.2.c</t>
-  </si>
-  <si>
-    <t>GCCGAGAAAGAAGATAATGAAGTGC</t>
+    <t>seg23.6.j.d</t>
+  </si>
+  <si>
+    <t>TGTTCCTGCTGACCTTCGTTC</t>
   </si>
   <si>
     <t>A07</t>
   </si>
   <si>
-    <t>seg23.3.d</t>
-  </si>
-  <si>
-    <t>AAACAAAGAAAGATACAGGCTGGAATAAG</t>
+    <t>seg23.7.j.d</t>
+  </si>
+  <si>
+    <t>GATTCAGCTGTAAACTCGCCAT</t>
   </si>
   <si>
     <t>A08</t>
   </si>
   <si>
-    <t>seg23.3.wt</t>
-  </si>
-  <si>
-    <t>AAACACAAAAAGATACAGGCTGGAATTAA</t>
-  </si>
-  <si>
-    <t>A09</t>
-  </si>
-  <si>
-    <t>seg23.3.c</t>
-  </si>
-  <si>
-    <t>GTATCCCACTCAGCCCTAATCG</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>seg23.4.d</t>
-  </si>
-  <si>
-    <t>CGTCATTGAATCCCAGTGCAG</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
-    <t>seg23.4.wt</t>
-  </si>
-  <si>
-    <t>CGTCATTGAATCCCAGTGCAC</t>
-  </si>
-  <si>
-    <t>A12</t>
-  </si>
-  <si>
-    <t>seg23.4.c</t>
-  </si>
-  <si>
-    <t>TCATAGTGAAACATATGCTTTAATGAATGTT</t>
-  </si>
-  <si>
-    <t>B01</t>
-  </si>
-  <si>
-    <t>seg23.5.d</t>
-  </si>
-  <si>
-    <t>AAGTCCACCGATATAAACACCTGTTGA</t>
-  </si>
-  <si>
-    <t>B02</t>
-  </si>
-  <si>
-    <t>seg23.5.wt</t>
-  </si>
-  <si>
-    <t>GAGACCACCGATATAAACACCTGTACT</t>
-  </si>
-  <si>
-    <t>B03</t>
-  </si>
-  <si>
-    <t>seg23.5.c</t>
-  </si>
-  <si>
-    <t>AATCATTATTCAGGGCAAAAACTCAT</t>
-  </si>
-  <si>
-    <t>B04</t>
-  </si>
-  <si>
-    <t>seg23.6.d</t>
-  </si>
-  <si>
-    <t>TTGTCAATTGAGATATTCGCACCT</t>
-  </si>
-  <si>
-    <t>B05</t>
-  </si>
-  <si>
-    <t>seg23.6.wt</t>
-  </si>
-  <si>
-    <t>TTGTCAATGCTGATATTCGCACCG</t>
-  </si>
-  <si>
-    <t>B06</t>
-  </si>
-  <si>
-    <t>seg23.6.c</t>
-  </si>
-  <si>
-    <t>CCTCTCCGGCAAAACTTAATCTG</t>
-  </si>
-  <si>
-    <t>B07</t>
-  </si>
-  <si>
-    <t>seg23.7.d</t>
-  </si>
-  <si>
-    <t>CGGACAACTGAAAAGGCTGATG</t>
-  </si>
-  <si>
-    <t>B08</t>
-  </si>
-  <si>
-    <t>seg23.7.wt</t>
-  </si>
-  <si>
-    <t>CGGACAACACTAAAGGCGCTAC</t>
-  </si>
-  <si>
-    <t>B09</t>
-  </si>
-  <si>
-    <t>seg23.7.c</t>
-  </si>
-  <si>
-    <t>ATTTTTTACATTTTCGATAAATTCATCTGCA</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
     <t>seg23.8.d</t>
   </si>
   <si>
-    <t>GTATCCAGCCCGTTATCATTCATTG</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>seg23.8.wt</t>
-  </si>
-  <si>
-    <t>GTATCCAGCCCGTTATCATTCATAC</t>
-  </si>
-  <si>
-    <t>B12</t>
+    <t>ATACAATTTGCGTGCCAGATTTTTATCTTTC</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>seg23.1.j.w</t>
+  </si>
+  <si>
+    <t>GACTTTTTACGCGGCAGATAAAATTTCTG</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>seg23.2.j.w</t>
+  </si>
+  <si>
+    <t>AGGAGTAAATAATGAACAAAGAGACACAACC</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>seg23.3.j.w</t>
+  </si>
+  <si>
+    <t>CGCTGGATTTTTGACTAAAGTTTCT</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>seg23.4.j.w</t>
+  </si>
+  <si>
+    <t>TCATCATTCTCAATCAGACAACTCTC</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>seg23.5.j.w</t>
+  </si>
+  <si>
+    <t>CATGACTTACAAATGCTTAGCCAATGG</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>seg23.6.j.w</t>
+  </si>
+  <si>
+    <t>TGTTCCTGCTGACCTTCGTTG</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>seg23.7.j.w</t>
+  </si>
+  <si>
+    <t>GAATCAGCTGTAACTGCGCCAG</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>seg23.8.w</t>
+  </si>
+  <si>
+    <t>ATACAATTTGCGTGCCAATTTTTTATCTTTT</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>seg23.1.j.c</t>
+  </si>
+  <si>
+    <t>GCTAATCTGGAACGTGACTGGTA</t>
+  </si>
+  <si>
+    <t>E02</t>
+  </si>
+  <si>
+    <t>seg23.2.j.c</t>
+  </si>
+  <si>
+    <t>TCCGCGAAGAGTTGAACGAA</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>seg23.3.j.c</t>
+  </si>
+  <si>
+    <t>GCTAGGCCCTTAACGGTTATT</t>
+  </si>
+  <si>
+    <t>E04</t>
+  </si>
+  <si>
+    <t>seg23.4.j.c</t>
+  </si>
+  <si>
+    <t>CCAGAAATGAATCATGGGGTATTTGAATAT</t>
+  </si>
+  <si>
+    <t>E05</t>
+  </si>
+  <si>
+    <t>seg23.5.j.c</t>
+  </si>
+  <si>
+    <t>AGCGGGAAATGACAGGCA</t>
+  </si>
+  <si>
+    <t>E06</t>
+  </si>
+  <si>
+    <t>seg23.6.j.c</t>
+  </si>
+  <si>
+    <t>GCGTAATCCCGGCAATCATC</t>
+  </si>
+  <si>
+    <t>E07</t>
+  </si>
+  <si>
+    <t>seg23.7.j.c</t>
+  </si>
+  <si>
+    <t>CCAGCGCGGATTGTTCCC</t>
+  </si>
+  <si>
+    <t>E08</t>
   </si>
   <si>
     <t>seg23.8.c</t>
   </si>
   <si>
-    <t>GCACAATCTACCTTCGAGCAAAAA</t>
+    <t>GCTGTTCGCCTCACCAAGT</t>
   </si>
 </sst>
 </file>

</xml_diff>